<commit_message>
Agregando el modod VV
</commit_message>
<xml_diff>
--- a/Benchmark.xlsx
+++ b/Benchmark.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Documents\2018-1\Visual\processing sketch\FlockOfBoids1 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36CA4BC-F7B6-4E88-B8A7-04F0F5A5E06C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F9187B-2E6E-4F6C-AFD6-503CC2768810}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{D26F3D28-74EC-4653-91DB-3258EC2E5C3A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="2" xr2:uid="{D26F3D28-74EC-4653-91DB-3258EC2E5C3A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Inmediato" sheetId="1" r:id="rId1"/>
+    <sheet name="F-V" sheetId="1" r:id="rId1"/>
+    <sheet name="V-V" sheetId="2" r:id="rId2"/>
+    <sheet name="Comparativa" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="6">
-  <si>
-    <t>Modo Inmediato</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="8">
   <si>
     <t>cantidad</t>
   </si>
@@ -42,7 +41,16 @@
     <t>Cantidad</t>
   </si>
   <si>
-    <t>Modo Retenido</t>
+    <t>Modo Inmediato V-V</t>
+  </si>
+  <si>
+    <t>Modo Retenido V-V</t>
+  </si>
+  <si>
+    <t>Modo Inmediato F-V</t>
+  </si>
+  <si>
+    <t>Modo Retenido F-V</t>
   </si>
 </sst>
 </file>
@@ -257,7 +265,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Inmediato!$B$4:$B$7</c:f>
+              <c:f>'F-V'!$B$4:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -278,7 +286,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Inmediato!$C$4:$C$7</c:f>
+              <c:f>'F-V'!$C$4:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -336,7 +344,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Inmediato!$B$17:$B$20</c:f>
+              <c:f>'F-V'!$B$17:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -357,7 +365,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Inmediato!$C$17:$C$20</c:f>
+              <c:f>'F-V'!$C$17:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -380,6 +388,1300 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-EE80-4ED4-87E2-76859DFF5468}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="468335968"/>
+        <c:axId val="468333016"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="468335968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-CO"/>
+                  <a:t>Cantidad</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-CO" baseline="0"/>
+                  <a:t> de nodos</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="468333016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="468333016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-CO"/>
+                  <a:t>Frame</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="468335968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1">
+          <a:alpha val="95000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CO" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>benchmark V-V </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-CO"/>
+              <a:t> </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>frameRateRetenido</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'V-V'!$B$17:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'V-V'!$C$17:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>60.085749899999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60.147666000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42.705252799999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.561912299999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E5DC-47F0-83F2-453A9AE540CD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>frameRateInmediato</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'V-V'!$B$4:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'V-V'!$C$4:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>60.229754499999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60.344426999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>49.723335200000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.524430599999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E5DC-47F0-83F2-453A9AE540CD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="468335968"/>
+        <c:axId val="468333016"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="468335968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-CO"/>
+                  <a:t>Cantidad</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-CO" baseline="0"/>
+                  <a:t> de nodos</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="468333016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="468333016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-CO"/>
+                  <a:t>Frame</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="468335968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1">
+          <a:alpha val="95000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CO" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>benchmark F-V y V-V </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-CO"/>
+              <a:t> </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>frameRateRetenidVV</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'V-V'!$B$17:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'V-V'!$C$17:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>60.085749899999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60.147666000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42.705252799999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.561912299999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-26BD-4EB4-A54B-85FFDEF1C635}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>frameRateInmediatoVV</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'V-V'!$B$4:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'V-V'!$C$4:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>60.229754499999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60.344426999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>49.723335200000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.524430599999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-26BD-4EB4-A54B-85FFDEF1C635}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>frameRateRetenidFV</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'F-V'!$B$17:$B$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'F-V'!$C$17:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>60.166463199999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60.419326699999985</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>49.959710800000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.650585999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-26BD-4EB4-A54B-85FFDEF1C635}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>frameRateInmediatoFV</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'F-V'!$B$4:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'F-V'!$C$4:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>60.532498700000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60.203899500000013</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>59.560074799999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.599638799999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-26BD-4EB4-A54B-85FFDEF1C635}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -754,7 +2056,1119 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1295,6 +3709,92 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D715C0D-ED76-4CBA-B4C4-48B0745A931F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>419099</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E3765FE-9BF1-4C7C-85F1-E87DC02C34CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1610,8 +4110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C265A1-D53D-44FB-97D6-1541AA8ADE60}">
   <dimension ref="B2:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1622,19 +4122,19 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C2" s="4"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3" s="1">
         <v>10</v>
@@ -1658,7 +4158,7 @@
         <v>60.532498700000005</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4" s="2">
         <v>60.289143000000003</v>
@@ -1682,7 +4182,7 @@
         <v>60.203899500000013</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" s="2">
         <v>65.471230000000006</v>
@@ -1706,7 +4206,7 @@
         <v>59.560074799999995</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6" s="2">
         <v>60.144703</v>
@@ -1730,7 +4230,7 @@
         <v>25.599638799999997</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7" s="2">
         <v>60.338431999999997</v>
@@ -1747,7 +4247,7 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E8" s="2">
         <v>60.233578000000001</v>
@@ -1764,7 +4264,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D9" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E9" s="2">
         <v>58.490948000000003</v>
@@ -1781,7 +4281,7 @@
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D10" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E10" s="2">
         <v>60.365012999999998</v>
@@ -1798,7 +4298,7 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D11" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E11" s="2">
         <v>59.986359999999998</v>
@@ -1815,7 +4315,7 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D12" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12" s="2">
         <v>60.10051</v>
@@ -1832,7 +4332,7 @@
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D13" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E13" s="2">
         <v>59.905070000000002</v>
@@ -1849,19 +4349,19 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C15" s="4"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="D16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E16" s="1">
         <v>10</v>
@@ -1885,7 +4385,7 @@
         <v>60.166463199999995</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E17" s="2">
         <v>60.189278000000002</v>
@@ -1909,7 +4409,7 @@
         <v>60.419326699999985</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E18" s="2">
         <v>60.626972000000002</v>
@@ -1933,7 +4433,7 @@
         <v>49.959710800000003</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E19" s="2">
         <v>60.264125999999997</v>
@@ -1957,7 +4457,7 @@
         <v>18.650585999999997</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E20" s="2">
         <v>59.904232</v>
@@ -1974,7 +4474,7 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D21" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E21" s="2">
         <v>60.129883</v>
@@ -1991,7 +4491,7 @@
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D22" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E22" s="2">
         <v>59.982146999999998</v>
@@ -2008,7 +4508,7 @@
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D23" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E23" s="2">
         <v>60.186332999999998</v>
@@ -2025,7 +4525,7 @@
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D24" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E24" s="2">
         <v>60.104709999999997</v>
@@ -2042,7 +4542,7 @@
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D25" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E25" s="2">
         <v>60.125686999999999</v>
@@ -2059,7 +4559,7 @@
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D26" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E26" s="2">
         <v>60.151263999999998</v>
@@ -2083,4 +4583,491 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CC08F25-936F-4470-899E-EDC8B7909BDF}">
+  <dimension ref="B2:H26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2">
+        <v>100</v>
+      </c>
+      <c r="G3" s="2">
+        <v>500</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1">
+        <f>SUM(E4:E13)/10</f>
+        <v>60.229754499999999</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>60.27272</v>
+      </c>
+      <c r="F4" s="2">
+        <v>60.136887000000002</v>
+      </c>
+      <c r="G4" s="2">
+        <v>42.082993000000002</v>
+      </c>
+      <c r="H4" s="2">
+        <v>23.470649999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>100</v>
+      </c>
+      <c r="C5" s="1">
+        <f>SUM(F4:F13)/10</f>
+        <v>60.344426999999996</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>60.124454</v>
+      </c>
+      <c r="F5" s="2">
+        <v>60.464385999999998</v>
+      </c>
+      <c r="G5" s="2">
+        <v>51.669795999999998</v>
+      </c>
+      <c r="H5" s="2">
+        <v>23.528207999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>500</v>
+      </c>
+      <c r="C6" s="1">
+        <f>SUM(G4:G13)/10</f>
+        <v>49.723335200000001</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>60.726930000000003</v>
+      </c>
+      <c r="F6" s="2">
+        <v>60.165260000000004</v>
+      </c>
+      <c r="G6" s="2">
+        <v>49.779494999999997</v>
+      </c>
+      <c r="H6" s="2">
+        <v>22.859712999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C7" s="1">
+        <f>SUM(H4:H13)/10</f>
+        <v>22.524430599999999</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>60.474274000000001</v>
+      </c>
+      <c r="F7" s="2">
+        <v>60.348537</v>
+      </c>
+      <c r="G7" s="2">
+        <v>49.797370000000001</v>
+      </c>
+      <c r="H7" s="2">
+        <v>21.754159999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>60.486519999999999</v>
+      </c>
+      <c r="F8" s="2">
+        <v>60.972790000000003</v>
+      </c>
+      <c r="G8" s="2">
+        <v>52.136620000000001</v>
+      </c>
+      <c r="H8" s="2">
+        <v>22.846541999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>60.055909999999997</v>
+      </c>
+      <c r="F9" s="2">
+        <v>60.141987</v>
+      </c>
+      <c r="G9" s="2">
+        <v>47.972670000000001</v>
+      </c>
+      <c r="H9" s="2">
+        <v>22.254867999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>60.037792000000003</v>
+      </c>
+      <c r="F10" s="2">
+        <v>60.478484999999999</v>
+      </c>
+      <c r="G10" s="2">
+        <v>50.251480000000001</v>
+      </c>
+      <c r="H10" s="2">
+        <v>22.625778</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="2">
+        <v>60.253017</v>
+      </c>
+      <c r="F11" s="2">
+        <v>60.270603000000001</v>
+      </c>
+      <c r="G11" s="2">
+        <v>50.207751999999999</v>
+      </c>
+      <c r="H11" s="2">
+        <v>21.7911</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="2">
+        <v>59.915362999999999</v>
+      </c>
+      <c r="F12" s="2">
+        <v>60.390590000000003</v>
+      </c>
+      <c r="G12" s="2">
+        <v>52.181865999999999</v>
+      </c>
+      <c r="H12" s="2">
+        <v>21.877516</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2">
+        <v>59.950564999999997</v>
+      </c>
+      <c r="F13" s="2">
+        <v>60.074745</v>
+      </c>
+      <c r="G13" s="2">
+        <v>51.153309999999998</v>
+      </c>
+      <c r="H13" s="2">
+        <v>22.235771</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="2">
+        <v>10</v>
+      </c>
+      <c r="F16" s="2">
+        <v>100</v>
+      </c>
+      <c r="G16" s="2">
+        <v>500</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <v>10</v>
+      </c>
+      <c r="C17" s="1">
+        <f>SUM(E17:E26)/10</f>
+        <v>60.085749899999996</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="2">
+        <v>59.987915000000001</v>
+      </c>
+      <c r="F17" s="2">
+        <v>60.039997</v>
+      </c>
+      <c r="G17" s="2">
+        <v>42.025300000000001</v>
+      </c>
+      <c r="H17" s="2">
+        <v>15.454373</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <v>100</v>
+      </c>
+      <c r="C18" s="1">
+        <f>SUM(F17:F26)/10</f>
+        <v>60.147666000000001</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="2">
+        <v>59.96116</v>
+      </c>
+      <c r="F18" s="2">
+        <v>59.951126000000002</v>
+      </c>
+      <c r="G18" s="2">
+        <v>45.134253999999999</v>
+      </c>
+      <c r="H18" s="2">
+        <v>14.994517</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>500</v>
+      </c>
+      <c r="C19" s="1">
+        <f>SUM(G17:G26)/10</f>
+        <v>42.705252799999997</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="2">
+        <v>59.637259999999998</v>
+      </c>
+      <c r="F19" s="2">
+        <v>60.216453999999999</v>
+      </c>
+      <c r="G19" s="2">
+        <v>40.489539999999998</v>
+      </c>
+      <c r="H19" s="2">
+        <v>14.807523</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C20" s="1">
+        <f>SUM(H17:H26)/10</f>
+        <v>15.561912299999999</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="2">
+        <v>59.820309999999999</v>
+      </c>
+      <c r="F20" s="2">
+        <v>60.166179999999997</v>
+      </c>
+      <c r="G20" s="2">
+        <v>43.708137999999998</v>
+      </c>
+      <c r="H20" s="2">
+        <v>16.090126000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="2">
+        <v>60.242713999999999</v>
+      </c>
+      <c r="F21" s="2">
+        <v>60.254455999999998</v>
+      </c>
+      <c r="G21" s="2">
+        <v>40.098373000000002</v>
+      </c>
+      <c r="H21" s="2">
+        <v>15.781685</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="2">
+        <v>60.192627000000002</v>
+      </c>
+      <c r="F22" s="2">
+        <v>60.339435999999999</v>
+      </c>
+      <c r="G22" s="2">
+        <v>43.171570000000003</v>
+      </c>
+      <c r="H22" s="2">
+        <v>15.212206999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="2">
+        <v>60.322754000000003</v>
+      </c>
+      <c r="F23" s="2">
+        <v>60.290751999999998</v>
+      </c>
+      <c r="G23" s="2">
+        <v>42.871482999999998</v>
+      </c>
+      <c r="H23" s="2">
+        <v>15.187447000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="2">
+        <v>60.271071999999997</v>
+      </c>
+      <c r="F24" s="2">
+        <v>60.318910000000002</v>
+      </c>
+      <c r="G24" s="2">
+        <v>42.720599999999997</v>
+      </c>
+      <c r="H24" s="2">
+        <v>16.056684000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="2">
+        <v>60.296579999999999</v>
+      </c>
+      <c r="F25" s="2">
+        <v>59.944026999999998</v>
+      </c>
+      <c r="G25" s="2">
+        <v>42.804389999999998</v>
+      </c>
+      <c r="H25" s="2">
+        <v>16.451826000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" s="2">
+        <v>60.125107</v>
+      </c>
+      <c r="F26" s="2">
+        <v>59.955322000000002</v>
+      </c>
+      <c r="G26" s="2">
+        <v>44.028880000000001</v>
+      </c>
+      <c r="H26" s="2">
+        <v>15.582735</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B15:C15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2145946E-C111-4A6D-B861-09DD88799865}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>